<commit_message>
Added halfway new Module
- Changed Address_3 field in Master Branch to Address_City
- Added Pengaturan Group Akses Module (Halfway Done)
- Added DB dumps for new tables (refer to dumpLog.xlsx)
- Added new field in Database Design
</commit_message>
<xml_diff>
--- a/_DBDUMPS_/dumpLog.xlsx
+++ b/_DBDUMPS_/dumpLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>FILENAME</t>
   </si>
@@ -26,6 +26,12 @@
   </si>
   <si>
     <t>first time dump from mysql, only contain MASTER_USER and MASTER_GROUP</t>
+  </si>
+  <si>
+    <t>Dump20160210</t>
+  </si>
+  <si>
+    <t>Added new tables (MASTER_BRANCH, MASTER_MODULE, USER_MANAGEMENT_ACCESS)</t>
   </si>
 </sst>
 </file>
@@ -76,9 +82,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,7 +395,7 @@
   <dimension ref="B4:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,8 +421,12 @@
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>

</xml_diff>

<commit_message>
Added DB Dump for UNIT_CONVERT Table
as per summary
</commit_message>
<xml_diff>
--- a/_DBDUMPS_/dumpLog.xlsx
+++ b/_DBDUMPS_/dumpLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>FILENAME</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Added new tables (MASTER_CATEGORY, MASTER_UNIT)</t>
+  </si>
+  <si>
+    <t>Dump20160214-1</t>
+  </si>
+  <si>
+    <t>Added new tables (UNIT_CONVERT)</t>
   </si>
 </sst>
 </file>
@@ -443,8 +449,12 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>

</xml_diff>

<commit_message>
Added new modules and tables
Master Supplier Module
Master Customer Module
Master Produk Module
</commit_message>
<xml_diff>
--- a/_DBDUMPS_/dumpLog.xlsx
+++ b/_DBDUMPS_/dumpLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>FILENAME</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Added new tables (MASTER_CUSTOMER, MASTER_SUPPLIER, MASTER_PRODUCT)</t>
+  </si>
+  <si>
+    <t>Dump20160217-1</t>
+  </si>
+  <si>
+    <t>Added new table (PRODUCT_CATEGORY)</t>
   </si>
 </sst>
 </file>
@@ -413,7 +419,7 @@
   <dimension ref="B4:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,8 +477,12 @@
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>

</xml_diff>

<commit_message>
Added new field on request table
</commit_message>
<xml_diff>
--- a/_DBDUMPS_/dumpLog.xlsx
+++ b/_DBDUMPS_/dumpLog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>FILENAME</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Added new table (PRODUCTS_MUTATION_HEADER, PRODUCTS_MUTATION_DETAIL)</t>
+  </si>
+  <si>
+    <t>Dump20160301</t>
+  </si>
+  <si>
+    <t>Added new field for REQUEST_ORDER_HEADER table</t>
   </si>
 </sst>
 </file>
@@ -440,7 +446,7 @@
   <dimension ref="A4:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,8 +539,12 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>

</xml_diff>